<commit_message>
changes with concurrent rate limit
</commit_message>
<xml_diff>
--- a/Traffic.xlsx
+++ b/Traffic.xlsx
@@ -439,7 +439,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -504,7 +504,7 @@
         <v>10</v>
       </c>
       <c r="H2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -530,7 +530,7 @@
         <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>